<commit_message>
File upload feature modification + added more data
</commit_message>
<xml_diff>
--- a/Data/Tables/ET2.xlsx
+++ b/Data/Tables/ET2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\GitHub\Training2\Data\NomineeModel\UserModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\Data\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D0C83C-BD94-43DF-A0B0-F16205FBFBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A4057F-D60F-46A1-8436-89B136B6235C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB97CE2-5848-4162-A957-04FDB820B051}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1095,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>200163</v>
+        <v>200940</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1171,7 +1171,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>200164</v>
+        <v>200941</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="V3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1247,7 +1247,7 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>200165</v>
+        <v>200942</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -1323,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>200166</v>
+        <v>200943</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="V5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>200167</v>
+        <v>200944</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="V6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -1475,7 +1475,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>200168</v>
+        <v>200945</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="V7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>23</v>
       </c>
       <c r="C8">
-        <v>200169</v>
+        <v>200946</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="V8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>200170</v>
+        <v>200947</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1703,7 +1703,7 @@
         <v>27</v>
       </c>
       <c r="C10">
-        <v>200171</v>
+        <v>200948</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="V10">
         <f t="shared" ref="V10:V64" ca="1" si="2">RANDBETWEEN(0,8-V3)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1779,7 +1779,7 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>200172</v>
+        <v>200949</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="V11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1855,7 +1855,7 @@
         <v>31</v>
       </c>
       <c r="C12">
-        <v>200173</v>
+        <v>200950</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="V12">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1931,7 +1931,7 @@
         <v>33</v>
       </c>
       <c r="C13">
-        <v>200174</v>
+        <v>200951</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="V13">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -2007,7 +2007,7 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>200175</v>
+        <v>200952</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="V14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -2083,7 +2083,7 @@
         <v>37</v>
       </c>
       <c r="C15">
-        <v>200176</v>
+        <v>200953</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="V15">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>39</v>
       </c>
       <c r="C16">
-        <v>200177</v>
+        <v>200954</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -2235,7 +2235,7 @@
         <v>41</v>
       </c>
       <c r="C17">
-        <v>200178</v>
+        <v>200955</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="V17">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>43</v>
       </c>
       <c r="C18">
-        <v>200179</v>
+        <v>200956</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="V18">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2387,7 +2387,7 @@
         <v>45</v>
       </c>
       <c r="C19">
-        <v>200180</v>
+        <v>200957</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="V19">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>47</v>
       </c>
       <c r="C20">
-        <v>200181</v>
+        <v>200958</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="V20">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -2539,7 +2539,7 @@
         <v>49</v>
       </c>
       <c r="C21">
-        <v>200182</v>
+        <v>200959</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="V21">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -2615,7 +2615,7 @@
         <v>51</v>
       </c>
       <c r="C22">
-        <v>200183</v>
+        <v>200960</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="V22">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -2691,7 +2691,7 @@
         <v>53</v>
       </c>
       <c r="C23">
-        <v>200184</v>
+        <v>200961</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="V23">
         <f ca="1">RANDBETWEEN(0,8-V16)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -2767,7 +2767,7 @@
         <v>55</v>
       </c>
       <c r="C24">
-        <v>200185</v>
+        <v>200962</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="V24">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>57</v>
       </c>
       <c r="C25">
-        <v>200186</v>
+        <v>200963</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="V25">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -2919,7 +2919,7 @@
         <v>59</v>
       </c>
       <c r="C26">
-        <v>200187</v>
+        <v>200964</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="V26">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -2995,7 +2995,7 @@
         <v>61</v>
       </c>
       <c r="C27">
-        <v>200188</v>
+        <v>200965</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="V27">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -3071,7 +3071,7 @@
         <v>63</v>
       </c>
       <c r="C28">
-        <v>200189</v>
+        <v>200966</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -3147,7 +3147,7 @@
         <v>65</v>
       </c>
       <c r="C29">
-        <v>200190</v>
+        <v>200967</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="V29">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W29">
         <v>0</v>
@@ -3223,7 +3223,7 @@
         <v>67</v>
       </c>
       <c r="C30">
-        <v>200191</v>
+        <v>200968</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="V30">
         <f ca="1">RANDBETWEEN(0,8-V23)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W30">
         <v>0</v>
@@ -3299,7 +3299,7 @@
         <v>69</v>
       </c>
       <c r="C31">
-        <v>200192</v>
+        <v>200969</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -3358,7 +3358,7 @@
       </c>
       <c r="V31">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W31">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>71</v>
       </c>
       <c r="C32">
-        <v>200193</v>
+        <v>200970</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="V32">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W32">
         <v>0</v>
@@ -3451,7 +3451,7 @@
         <v>73</v>
       </c>
       <c r="C33">
-        <v>200194</v>
+        <v>200971</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="V33">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W33">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         <v>75</v>
       </c>
       <c r="C34">
-        <v>200195</v>
+        <v>200972</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="V34">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W34">
         <v>0</v>
@@ -3603,7 +3603,7 @@
         <v>77</v>
       </c>
       <c r="C35">
-        <v>200196</v>
+        <v>200973</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -3679,7 +3679,7 @@
         <v>79</v>
       </c>
       <c r="C36">
-        <v>200197</v>
+        <v>200974</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="V36">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W36">
         <v>0</v>
@@ -3755,7 +3755,7 @@
         <v>81</v>
       </c>
       <c r="C37">
-        <v>200198</v>
+        <v>200975</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="V37">
         <f ca="1">RANDBETWEEN(0,8-V30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W37">
         <v>0</v>
@@ -3831,7 +3831,7 @@
         <v>83</v>
       </c>
       <c r="C38">
-        <v>200199</v>
+        <v>200976</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="V38">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W38">
         <v>0</v>
@@ -3907,7 +3907,7 @@
         <v>85</v>
       </c>
       <c r="C39">
-        <v>200200</v>
+        <v>200977</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="V39">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W39">
         <v>0</v>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
       <c r="C40">
-        <v>200201</v>
+        <v>200978</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="V40">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W40">
         <v>0</v>
@@ -4059,7 +4059,7 @@
         <v>89</v>
       </c>
       <c r="C41">
-        <v>200202</v>
+        <v>200979</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -4135,7 +4135,7 @@
         <v>91</v>
       </c>
       <c r="C42">
-        <v>200203</v>
+        <v>200980</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -4211,7 +4211,7 @@
         <v>93</v>
       </c>
       <c r="C43">
-        <v>200204</v>
+        <v>200981</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="V43">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W43">
         <v>0</v>
@@ -4287,7 +4287,7 @@
         <v>95</v>
       </c>
       <c r="C44">
-        <v>200205</v>
+        <v>200982</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="V44">
         <f ca="1">RANDBETWEEN(0,8-V37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44">
         <v>0</v>
@@ -4363,7 +4363,7 @@
         <v>97</v>
       </c>
       <c r="C45">
-        <v>200206</v>
+        <v>200983</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="V45">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W45">
         <v>0</v>
@@ -4439,7 +4439,7 @@
         <v>99</v>
       </c>
       <c r="C46">
-        <v>200207</v>
+        <v>200984</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="V46">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W46">
         <v>0</v>
@@ -4515,7 +4515,7 @@
         <v>101</v>
       </c>
       <c r="C47">
-        <v>200208</v>
+        <v>200985</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="V47">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W47">
         <v>0</v>
@@ -4591,7 +4591,7 @@
         <v>103</v>
       </c>
       <c r="C48">
-        <v>200209</v>
+        <v>200986</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="V48">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W48">
         <v>0</v>
@@ -4667,7 +4667,7 @@
         <v>105</v>
       </c>
       <c r="C49">
-        <v>200210</v>
+        <v>200987</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="V49">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="W49">
         <v>0</v>
@@ -4743,7 +4743,7 @@
         <v>107</v>
       </c>
       <c r="C50">
-        <v>200211</v>
+        <v>200988</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -4802,7 +4802,7 @@
       </c>
       <c r="V50">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W50">
         <v>0</v>
@@ -4819,7 +4819,7 @@
         <v>109</v>
       </c>
       <c r="C51">
-        <v>200212</v>
+        <v>200989</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
@@ -4895,7 +4895,7 @@
         <v>111</v>
       </c>
       <c r="C52">
-        <v>200213</v>
+        <v>200990</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="V52">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W52">
         <v>0</v>
@@ -4971,7 +4971,7 @@
         <v>113</v>
       </c>
       <c r="C53">
-        <v>200214</v>
+        <v>200991</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="V53">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W53">
         <v>0</v>
@@ -5047,7 +5047,7 @@
         <v>115</v>
       </c>
       <c r="C54">
-        <v>200215</v>
+        <v>200992</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="V54">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W54">
         <v>0</v>
@@ -5123,7 +5123,7 @@
         <v>117</v>
       </c>
       <c r="C55">
-        <v>200216</v>
+        <v>200993</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="V55">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W55">
         <v>0</v>
@@ -5199,7 +5199,7 @@
         <v>119</v>
       </c>
       <c r="C56">
-        <v>200217</v>
+        <v>200994</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="V56">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W56">
         <v>0</v>
@@ -5275,7 +5275,7 @@
         <v>121</v>
       </c>
       <c r="C57">
-        <v>200218</v>
+        <v>200995</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="V57">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W57">
         <v>0</v>
@@ -5351,7 +5351,7 @@
         <v>123</v>
       </c>
       <c r="C58">
-        <v>200219</v>
+        <v>200996</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="V58">
         <f ca="1">RANDBETWEEN(0,8-V51)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W58">
         <v>0</v>
@@ -5427,7 +5427,7 @@
         <v>125</v>
       </c>
       <c r="C59">
-        <v>200220</v>
+        <v>200997</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="V59">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W59">
         <v>0</v>
@@ -5503,7 +5503,7 @@
         <v>127</v>
       </c>
       <c r="C60">
-        <v>200221</v>
+        <v>200998</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
@@ -5579,7 +5579,7 @@
         <v>129</v>
       </c>
       <c r="C61">
-        <v>200222</v>
+        <v>200999</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
@@ -5638,7 +5638,7 @@
       </c>
       <c r="V61">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W61">
         <v>0</v>
@@ -5655,7 +5655,7 @@
         <v>131</v>
       </c>
       <c r="C62">
-        <v>200223</v>
+        <v>201000</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -5731,7 +5731,7 @@
         <v>133</v>
       </c>
       <c r="C63">
-        <v>200224</v>
+        <v>201001</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="V63">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W63">
         <v>0</v>
@@ -5807,7 +5807,7 @@
         <v>135</v>
       </c>
       <c r="C64">
-        <v>200225</v>
+        <v>201002</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="V64">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W64">
         <v>0</v>

</xml_diff>